<commit_message>
Daylirate is store as a String
</commit_message>
<xml_diff>
--- a/trunk/management-v/ManagementVinci/Vinci Request.xlsx
+++ b/trunk/management-v/ManagementVinci/Vinci Request.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Toujours des problèmes de performances quand on tape du texte</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t>Il faudrait rajouter la possibilité de mettre du texte pour les Daily rate pour qu’on puisse mettre le type de monnaie</t>
   </si>
 </sst>
 </file>
@@ -164,19 +167,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -199,18 +189,39 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -223,7 +234,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -239,10 +252,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -252,9 +265,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -267,9 +278,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -284,19 +293,19 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -604,64 +613,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="1"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="11"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="2"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1">
-      <c r="A8" s="7" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>